<commit_message>
Yabla de datos vc
</commit_message>
<xml_diff>
--- a/Docs/VC- Tablas de Datos Lab 7.xlsx
+++ b/Docs/VC- Tablas de Datos Lab 7.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="23801"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10323"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://uniandes.sharepoint.com/sites/ISIS1225/Documentos compartidos/General/202110/Laboratorios/Lab 07 - Colisiones/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/valentina/Desktop/EDA - Lab/-LabCollision-S07-G04-/Docs/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="511" documentId="8_{A25BB2A9-7879-4ABF-A93E-5BD797619927}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{5A6E5986-5D76-40E6-8BB6-4E7550720C79}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F1672C0D-C967-014C-89C5-92CC06B4BBBA}" xr6:coauthVersionLast="46" xr6:coauthVersionMax="46" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-2127" yWindow="7073" windowWidth="4267" windowHeight="2354" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
+    <workbookView xWindow="3860" yWindow="500" windowWidth="24140" windowHeight="17500" tabRatio="767" xr2:uid="{D82936D8-D2C9-4EB2-9CBC-3665F65B95FD}"/>
   </bookViews>
   <sheets>
     <sheet name="Datos Lab7" sheetId="1" r:id="rId1"/>
@@ -97,18 +97,39 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFD9D9D9"/>
+        <bgColor rgb="FFD9D9D9"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-0.14999847407452621"/>
+        <bgColor theme="0" tint="-0.14999847407452621"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="1">
+  <borders count="2">
     <border>
       <left/>
       <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
       <top/>
       <bottom/>
       <diagonal/>
@@ -117,18 +138,30 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="2" fontId="1" fillId="2" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
@@ -161,6 +194,14 @@
         </patternFill>
       </fill>
       <alignment horizontal="center" vertical="center" textRotation="0" wrapText="1" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color indexed="64"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
     </dxf>
     <dxf>
       <font>
@@ -408,7 +449,7 @@
 <file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
   <c:date1904 val="0"/>
-  <c:lang val="en-US"/>
+  <c:lang val="es-MX"/>
   <c:roundedCorners val="0"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
@@ -481,7 +522,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:title>
@@ -568,7 +609,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -580,13 +621,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1324009.838</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>105</c:v>
+                  <c:v>1324009.838</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>115</c:v>
+                  <c:v>1324009.838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -598,13 +639,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>45</c:v>
+                  <c:v>43252.578666666668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>55</c:v>
+                  <c:v>42742.973333333335</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>75</c:v>
+                  <c:v>43873.407999999996</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -694,7 +735,7 @@
                       <a:cs typeface="+mn-cs"/>
                     </a:defRPr>
                   </a:pPr>
-                  <a:endParaRPr lang="en-US"/>
+                  <a:endParaRPr lang="es-CO"/>
                 </a:p>
               </c:txPr>
             </c:trendlineLbl>
@@ -706,13 +747,13 @@
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
                 <c:pt idx="0">
-                  <c:v>100</c:v>
+                  <c:v>1324009.838</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>120</c:v>
+                  <c:v>1324009.838</c:v>
                 </c:pt>
-                <c:pt idx="2">
-                  <c:v>140</c:v>
+                <c:pt idx="2" formatCode="General">
+                  <c:v>1324009.838</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -723,14 +764,14 @@
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="3"/>
-                <c:pt idx="0">
-                  <c:v>90</c:v>
+                <c:pt idx="0" formatCode="General">
+                  <c:v>45344.06966666667</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>100</c:v>
+                  <c:v>46411.244000000006</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>110</c:v>
+                  <c:v>46841.351333333332</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -835,7 +876,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -873,7 +914,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="1833162896"/>
@@ -957,7 +998,7 @@
                   <a:cs typeface="+mn-cs"/>
                 </a:defRPr>
               </a:pPr>
-              <a:endParaRPr lang="en-US"/>
+              <a:endParaRPr lang="es-CO"/>
             </a:p>
           </c:txPr>
         </c:title>
@@ -995,7 +1036,7 @@
                 <a:cs typeface="+mn-cs"/>
               </a:defRPr>
             </a:pPr>
-            <a:endParaRPr lang="en-US"/>
+            <a:endParaRPr lang="es-CO"/>
           </a:p>
         </c:txPr>
         <c:crossAx val="696671312"/>
@@ -1037,7 +1078,7 @@
               <a:cs typeface="+mn-cs"/>
             </a:defRPr>
           </a:pPr>
-          <a:endParaRPr lang="en-US"/>
+          <a:endParaRPr lang="es-CO"/>
         </a:p>
       </c:txPr>
     </c:legend>
@@ -1074,7 +1115,7 @@
       <a:pPr>
         <a:defRPr/>
       </a:pPr>
-      <a:endParaRPr lang="en-US"/>
+      <a:endParaRPr lang="es-CO"/>
     </a:p>
   </c:txPr>
 </c:chartSpace>
@@ -1648,7 +1689,7 @@
 <xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
   <xdr:absoluteAnchor>
     <xdr:pos x="0" y="0"/>
-    <xdr:ext cx="8661768" cy="6283739"/>
+    <xdr:ext cx="8669130" cy="6272696"/>
     <xdr:graphicFrame macro="">
       <xdr:nvGraphicFramePr>
         <xdr:cNvPr id="2" name="Chart 1">
@@ -1678,31 +1719,39 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{072D0253-75B0-4C0B-8972-D03303899249}" name="Table1" displayName="Table1" ref="A2:C5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
-  <autoFilter ref="A2:C5" xr:uid="{B245DDE7-54F2-4A7A-AC17-5CA17DD7B03F}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{873D9865-3B51-3A44-93F0-BE36C5A19588}" name="Table14" displayName="Table14" ref="A2:C5" totalsRowShown="0" headerRowDxfId="9" dataDxfId="8">
+  <autoFilter ref="A2:C5" xr:uid="{C0E39E31-4389-4A4E-A737-4CA072A4B477}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{A7AF2A2F-BC4B-404E-9B8B-256DA178E68B}" name="Factor de Carga (PROBING)" dataDxfId="7"/>
-    <tableColumn id="2" xr3:uid="{23CECC62-35E0-466E-9502-4F5CC2E6F7A7}" name="Consumo de Datos [kB]" dataDxfId="6"/>
-    <tableColumn id="3" xr3:uid="{19B1D273-887B-4392-991E-015D36D99E5B}" name="Tiempo de Ejecución [ms]" dataDxfId="5"/>
+    <tableColumn id="1" xr3:uid="{D7AB8460-42AD-D044-B09C-7CB7432920B7}" name="Factor de Carga (PROBING)" dataDxfId="7"/>
+    <tableColumn id="2" xr3:uid="{107D11EB-FEF2-474B-9A7F-66021BC7246A}" name="Consumo de Datos [kB]" dataDxfId="6">
+      <calculatedColumnFormula>AVERAGE(1324030.727,1323999.429,1323999.358)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{8335926F-E555-1547-B5B0-50A2D3FDB015}" name="Tiempo de Ejecución [ms]" dataDxfId="5">
+      <calculatedColumnFormula>AVERAGE(40695.658,28954.351,33240.404,32154.696)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{C35EFFA4-2B65-46C5-8257-6884800B9577}" name="Table13" displayName="Table13" ref="A9:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
-  <autoFilter ref="A9:C12" xr:uid="{5C24B5A8-1B8E-4092-B34A-66FF5413D106}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{EED9731F-5E3D-3D4B-B9A5-322A3B3A58BC}" name="Table135" displayName="Table135" ref="A9:C12" totalsRowShown="0" headerRowDxfId="4" dataDxfId="3">
+  <autoFilter ref="A9:C12" xr:uid="{8127B0BB-7521-1A4A-8BE1-29F2199569B5}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{16584851-71BC-4FF5-B248-C3F46BA653AF}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{4F9B7329-040C-4D35-96E7-B9181424DC65}" name="Consumo de Datos [kB]" dataDxfId="1"/>
-    <tableColumn id="3" xr3:uid="{BDA028DF-4CED-4928-B040-96AD8F8A43EB}" name="Tiempo de Ejecución [ms]" dataDxfId="0"/>
+    <tableColumn id="1" xr3:uid="{05E3E8C8-553D-DE43-A37E-442B6B3D5912}" name="Factor de Carga (CHAINING)" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{269F4831-4803-954E-9BB6-44C17AF6361E}" name="Consumo de Datos [kB]" dataDxfId="1">
+      <calculatedColumnFormula>AVERAGE(1324030.727,1323999.429,1323999.358)</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{4EDFC865-D4D0-5F46-81CA-03540D258E0B}" name="Tiempo de Ejecución [ms]" dataDxfId="0">
+      <calculatedColumnFormula>AVERAGE(35756.639,31360.055,29879.004,30473.106)</calculatedColumnFormula>
+    </tableColumn>
   </tableColumns>
   <tableStyleInfo name="TableStyleLight1" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
-<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Office Theme">
+<a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Tema de Office">
   <a:themeElements>
     <a:clrScheme name="Office">
       <a:dk1>
@@ -2001,119 +2050,149 @@
   <dimension ref="A1:C21"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B25" sqref="B25"/>
+      <selection activeCell="D25" sqref="D25"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.35" x14ac:dyDescent="0.5"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="27.64453125" style="3" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="26.05859375" style="3" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="25.8203125" style="3" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="27.6640625" style="1" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="29.83203125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="25.83203125" style="1" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A1" s="4" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
         <v>3</v>
       </c>
-      <c r="B1" s="4"/>
-      <c r="C1" s="4"/>
+      <c r="B1" s="7"/>
+      <c r="C1" s="7"/>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A2" s="2" t="s">
         <v>0</v>
       </c>
-      <c r="B2" s="1" t="s">
+      <c r="B2" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C2" s="1" t="s">
+      <c r="C2" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A3" s="2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="3">
         <v>0.3</v>
       </c>
-      <c r="B3" s="2">
-        <v>100</v>
-      </c>
-      <c r="C3" s="2">
-        <v>45</v>
+      <c r="B3" s="4">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C3" s="3">
+        <f>AVERAGE(46465.032,42114.378,41178.326)</f>
+        <v>43252.578666666668</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A4" s="2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="3">
         <v>0.5</v>
       </c>
-      <c r="B4" s="2">
-        <v>105</v>
-      </c>
-      <c r="C4" s="2">
-        <v>55</v>
+      <c r="B4" s="3">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C4" s="3">
+        <f>AVERAGE(47695.141,40702.637,39831.142)</f>
+        <v>42742.973333333335</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A5" s="2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="3">
         <v>0.8</v>
       </c>
-      <c r="B5" s="2">
-        <v>115</v>
-      </c>
-      <c r="C5" s="2">
-        <v>75</v>
+      <c r="B5" s="3">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C5" s="3">
+        <f>AVERAGE(48240.601,42357.221,41022.402)</f>
+        <v>43873.407999999996</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A8" s="4" t="s">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="5"/>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="5"/>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="7" t="s">
         <v>4</v>
       </c>
-      <c r="B8" s="4"/>
-      <c r="C8" s="4"/>
+      <c r="B8" s="7"/>
+      <c r="C8" s="7"/>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A9" s="1" t="s">
+    <row r="9" spans="1:3" ht="16" x14ac:dyDescent="0.2">
+      <c r="A9" s="2" t="s">
         <v>1</v>
       </c>
-      <c r="B9" s="1" t="s">
+      <c r="B9" s="2" t="s">
         <v>5</v>
       </c>
-      <c r="C9" s="1" t="s">
+      <c r="C9" s="2" t="s">
         <v>2</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A10" s="2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A10" s="3">
         <v>2</v>
       </c>
-      <c r="B10" s="2">
-        <v>100</v>
-      </c>
-      <c r="C10" s="2">
-        <v>90</v>
+      <c r="B10" s="3">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C10" s="8">
+        <f>AVERAGE(47514.284,41701.165,46816.76)</f>
+        <v>45344.06966666667</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A11" s="2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A11" s="3">
         <v>4</v>
       </c>
-      <c r="B11" s="2">
-        <v>120</v>
-      </c>
-      <c r="C11" s="2">
-        <v>100</v>
+      <c r="B11" s="3">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C11" s="6">
+        <f>AVERAGE(52250.555,42442.392,44540.785)</f>
+        <v>46411.244000000006</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.5">
-      <c r="A12" s="2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A12" s="3">
         <v>6</v>
       </c>
-      <c r="B12" s="2">
-        <v>140</v>
-      </c>
-      <c r="C12" s="2">
-        <v>110</v>
+      <c r="B12" s="5">
+        <f>AVERAGE(1324030.727,1323999.429,1323999.358)</f>
+        <v>1324009.838</v>
+      </c>
+      <c r="C12" s="6">
+        <f>AVERAGE(48494.584,42446.265,49583.205)</f>
+        <v>46841.351333333332</v>
       </c>
     </row>
-    <row r="21" ht="14.7" customHeight="1" x14ac:dyDescent="0.5"/>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A13" s="5"/>
+      <c r="B13" s="5"/>
+      <c r="C13" s="5"/>
+    </row>
+    <row r="19" spans="3:3" x14ac:dyDescent="0.2">
+      <c r="C19" s="8"/>
+    </row>
+    <row r="21" spans="3:3" ht="14.75" customHeight="1" x14ac:dyDescent="0.2"/>
   </sheetData>
   <mergeCells count="2">
     <mergeCell ref="A1:C1"/>
@@ -2128,6 +2207,12 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement/>
+</p:properties>
+</file>
+
+<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
 <ct:contentTypeSchema xmlns:ct="http://schemas.microsoft.com/office/2006/metadata/contentType" xmlns:ma="http://schemas.microsoft.com/office/2006/metadata/properties/metaAttributes" ct:_="" ma:_="" ma:contentTypeName="Documento" ma:contentTypeID="0x01010023858CF01A2EF24688B692775F4C60A4" ma:contentTypeVersion="11" ma:contentTypeDescription="Crear nuevo documento." ma:contentTypeScope="" ma:versionID="04b510ef1bc187d79b842c792d256c41">
   <xsd:schema xmlns:xsd="http://www.w3.org/2001/XMLSchema" xmlns:xs="http://www.w3.org/2001/XMLSchema" xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:ns2="164883f8-7691-4ecf-b54a-664c0d0edefe" xmlns:ns3="85e30bcc-d76c-4413-8e4d-2dce22fb0743" targetNamespace="http://schemas.microsoft.com/office/2006/metadata/properties" ma:root="true" ma:fieldsID="9049981c3eb1ee76226ec9e2f8ecd7b4" ns2:_="" ns3:_="">
     <xsd:import namespace="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
@@ -2338,12 +2423,6 @@
 </ct:contentTypeSchema>
 </file>
 
-<file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement/>
-</p:properties>
-</file>
-
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
 <?mso-contentType ?>
 <FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
@@ -2354,6 +2433,23 @@
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
+  <ds:schemaRefs>
+    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+  </ds:schemaRefs>
+</ds:datastoreItem>
+</file>
+
+<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{93C2AFC4-FCA8-4617-A6BD-EF7AAAEEB795}">
   <ds:schemaRefs>
     <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/contentType"/>
@@ -2372,23 +2468,6 @@
 </ds:datastoreItem>
 </file>
 
-<file path=customXml/itemProps2.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{97C5E1E0-C817-4769-9D2D-1DC296B681FA}">
-  <ds:schemaRefs>
-    <ds:schemaRef ds:uri="164883f8-7691-4ecf-b54a-664c0d0edefe"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="85e30bcc-d76c-4413-8e4d-2dce22fb0743"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
-  </ds:schemaRefs>
-</ds:datastoreItem>
-</file>
-
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
 <ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{F8DF3742-38F2-4B99-B335-CC4F04ED9F45}">
   <ds:schemaRefs>

</xml_diff>